<commit_message>
add daily comsumption 1.11-1.18
</commit_message>
<xml_diff>
--- a/accout.xlsx
+++ b/accout.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$207</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -174,6 +174,114 @@
   </si>
   <si>
     <t>标记</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>咖啡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>未知</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生活</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中餐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打针</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>菜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>超市</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交通</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外卖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>城际高铁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>菜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>买药</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>城际高铁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>滴滴打车</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>栗子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>超市</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>京东</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>摩拜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>早餐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>麻辣烫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蛋糕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>零食</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>盐酥鸡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电影票</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>午餐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>餐费</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地铁</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -337,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -360,11 +468,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -672,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2656"/>
+  <dimension ref="A1:D2812"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -699,7 +813,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="19" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -713,7 +827,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" s="15"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
@@ -725,7 +839,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="15"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
@@ -737,7 +851,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="15"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -749,7 +863,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" s="15"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
@@ -761,7 +875,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="15"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
@@ -773,7 +887,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="15"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
@@ -785,8 +899,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16" t="s">
+      <c r="A9" s="19"/>
+      <c r="B9" s="20" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="5">
@@ -797,8 +911,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="5">
         <v>20.5</v>
       </c>
@@ -807,8 +921,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="5">
         <v>22.72</v>
       </c>
@@ -817,7 +931,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" s="15"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="5" t="s">
         <v>13</v>
       </c>
@@ -829,7 +943,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="15"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
@@ -841,7 +955,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A14" s="15"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
@@ -853,7 +967,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="15"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="5" t="s">
         <v>16</v>
       </c>
@@ -865,7 +979,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="15"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -877,7 +991,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="15"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="5" t="s">
         <v>18</v>
       </c>
@@ -889,7 +1003,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="15"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="5" t="s">
         <v>19</v>
       </c>
@@ -901,7 +1015,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="15"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="5" t="s">
         <v>20</v>
       </c>
@@ -913,7 +1027,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="15"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="5" t="s">
         <v>21</v>
       </c>
@@ -925,7 +1039,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="15"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="5" t="s">
         <v>22</v>
       </c>
@@ -937,7 +1051,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="15"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="5" t="s">
         <v>20</v>
       </c>
@@ -949,7 +1063,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="15"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="5" t="s">
         <v>23</v>
       </c>
@@ -961,7 +1075,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="15"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="5" t="s">
         <v>24</v>
       </c>
@@ -973,7 +1087,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="15"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="5" t="s">
         <v>25</v>
       </c>
@@ -985,10 +1099,10 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="15">
+      <c r="A26" s="19">
         <v>1.9</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="20" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="5">
@@ -999,8 +1113,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="15"/>
-      <c r="B27" s="16"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="20"/>
       <c r="C27" s="5">
         <v>28.8</v>
       </c>
@@ -1009,11 +1123,11 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="15"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="17">
+      <c r="C28" s="16">
         <v>50.16</v>
       </c>
       <c r="D28" s="6">
@@ -1021,7 +1135,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="15"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="5" t="s">
         <v>4</v>
       </c>
@@ -1033,51 +1147,51 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="20">
+      <c r="A30" s="22">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="17">
+      <c r="C30" s="16">
         <v>41.26</v>
       </c>
-      <c r="D30" s="18">
+      <c r="D30" s="17">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A31" s="20"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="17">
+      <c r="A31" s="22"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="16">
         <v>13</v>
       </c>
-      <c r="D31" s="18">
+      <c r="D31" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A32" s="20"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="17">
+      <c r="A32" s="22"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="16">
         <v>15</v>
       </c>
-      <c r="D32" s="18">
+      <c r="D32" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A33" s="20"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="17">
+      <c r="A33" s="22"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="16">
         <v>39</v>
       </c>
-      <c r="D33" s="18">
+      <c r="D33" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="20"/>
+      <c r="A34" s="22"/>
       <c r="B34" t="s">
         <v>32</v>
       </c>
@@ -1089,7 +1203,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="20"/>
+      <c r="A35" s="22"/>
       <c r="B35" t="s">
         <v>33</v>
       </c>
@@ -1101,7 +1215,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="20"/>
+      <c r="A36" s="22"/>
       <c r="B36" t="s">
         <v>34</v>
       </c>
@@ -1113,7 +1227,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="20"/>
+      <c r="A37" s="22"/>
       <c r="B37" t="s">
         <v>35</v>
       </c>
@@ -1125,7 +1239,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="20"/>
+      <c r="A38" s="22"/>
       <c r="B38" t="s">
         <v>37</v>
       </c>
@@ -1136,101 +1250,1282 @@
         <v>1</v>
       </c>
     </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A39" s="18">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="B39" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39">
+        <v>6</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A40" s="4"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="6"/>
+      <c r="A40" s="18"/>
+      <c r="B40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40">
+        <v>26.36</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="4"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="6"/>
+      <c r="A41" s="18"/>
+      <c r="B41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <v>28</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A42" s="4"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="6"/>
+      <c r="A42" s="18"/>
+      <c r="B42" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <v>48</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="4"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="6"/>
+      <c r="A43" s="18"/>
+      <c r="B43" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43">
+        <v>10.5</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="4"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="6"/>
+      <c r="A44" s="18"/>
+      <c r="B44" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44">
+        <v>127</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="4"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="6"/>
+      <c r="A45" s="18"/>
+      <c r="B45" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45">
+        <v>25</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="4"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="6"/>
+      <c r="A46" s="18">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="B46" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46">
+        <v>27.84</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="4"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="6"/>
+      <c r="A47" s="18"/>
+      <c r="B47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="18"/>
+      <c r="B48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48">
+        <v>20</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A49" s="18"/>
+      <c r="B49" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49">
+        <v>24.5</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A50" s="18">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="B50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50">
+        <v>54.5</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A51" s="18"/>
+      <c r="B51" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51">
+        <v>53.58</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A52" s="18"/>
+      <c r="B52" t="s">
+        <v>49</v>
+      </c>
+      <c r="C52">
+        <v>21.42</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A53" s="18"/>
+      <c r="B53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>39</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A54" s="18"/>
+      <c r="B54" t="s">
+        <v>50</v>
+      </c>
+      <c r="C54">
+        <v>81</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A55" s="18">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="B55" t="s">
+        <v>51</v>
+      </c>
+      <c r="C55">
+        <v>54.5</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A56" s="18"/>
+      <c r="B56" t="s">
+        <v>52</v>
+      </c>
+      <c r="C56">
+        <v>12.63</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A57" s="18"/>
+      <c r="B57" t="s">
+        <v>53</v>
+      </c>
+      <c r="C57">
+        <v>25</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A58" s="18">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="B58" t="s">
+        <v>54</v>
+      </c>
+      <c r="C58">
+        <v>42.5</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A59" s="18">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="B59" t="s">
+        <v>55</v>
+      </c>
+      <c r="C59">
+        <v>35.9</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A60" s="18"/>
+      <c r="B60" t="s">
+        <v>56</v>
+      </c>
+      <c r="C60">
+        <v>12</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A61" s="18"/>
+      <c r="B61" t="s">
+        <v>44</v>
+      </c>
+      <c r="C61">
+        <v>86.63</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A62" s="18"/>
+      <c r="B62" t="s">
+        <v>57</v>
+      </c>
+      <c r="C62">
+        <v>5</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A63" s="18"/>
+      <c r="B63" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63">
+        <v>26</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A64" s="18">
+        <v>1.17</v>
+      </c>
+      <c r="B64" t="s">
+        <v>44</v>
+      </c>
+      <c r="C64">
+        <v>84</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A65" s="18"/>
+      <c r="B65" t="s">
+        <v>57</v>
+      </c>
+      <c r="C65">
+        <v>5</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B66" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66">
+        <v>17</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A67" s="4"/>
+      <c r="B67" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C67" s="5">
         <v>27</v>
       </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2">
+      <c r="D67" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A68" s="4">
+        <v>1.18</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C68" s="16">
+        <v>30</v>
+      </c>
+      <c r="D68" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A69" s="4"/>
+      <c r="B69" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C69" s="16">
+        <v>21.5</v>
+      </c>
+      <c r="D69" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A70" s="4"/>
+      <c r="B70" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C70" s="16">
+        <v>17</v>
+      </c>
+      <c r="D70" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A71" s="4"/>
+      <c r="B71" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C71" s="16">
+        <v>10</v>
+      </c>
+      <c r="D71" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A72" s="15"/>
+      <c r="B72" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C72" s="16">
+        <v>400</v>
+      </c>
+      <c r="D72" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A73" s="4"/>
+      <c r="B73" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C73" s="16">
+        <v>100</v>
+      </c>
+      <c r="D73" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A74" s="4"/>
+      <c r="B74" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C74" s="16">
+        <v>80</v>
+      </c>
+      <c r="D74" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A75" s="15"/>
+      <c r="B75" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C75" s="16">
+        <v>4</v>
+      </c>
+      <c r="D75" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A76" s="15"/>
+      <c r="B76" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C76" s="16"/>
+      <c r="D76" s="6"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A77" s="15"/>
+      <c r="B77" s="16"/>
+      <c r="C77" s="16"/>
+      <c r="D77" s="6"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A78" s="15"/>
+      <c r="B78" s="16"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="6"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A79" s="15"/>
+      <c r="B79" s="16"/>
+      <c r="C79" s="16"/>
+      <c r="D79" s="6"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A80" s="15"/>
+      <c r="B80" s="16"/>
+      <c r="C80" s="16"/>
+      <c r="D80" s="6"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A81" s="15"/>
+      <c r="B81" s="16"/>
+      <c r="C81" s="16"/>
+      <c r="D81" s="6"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A82" s="15"/>
+      <c r="B82" s="16"/>
+      <c r="C82" s="16"/>
+      <c r="D82" s="6"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A83" s="15"/>
+      <c r="B83" s="16"/>
+      <c r="C83" s="16"/>
+      <c r="D83" s="6"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A84" s="15"/>
+      <c r="B84" s="16"/>
+      <c r="C84" s="16"/>
+      <c r="D84" s="6"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A85" s="15"/>
+      <c r="B85" s="16"/>
+      <c r="C85" s="16"/>
+      <c r="D85" s="6"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A86" s="15"/>
+      <c r="B86" s="16"/>
+      <c r="C86" s="16"/>
+      <c r="D86" s="6"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A87" s="15"/>
+      <c r="B87" s="16"/>
+      <c r="C87" s="16"/>
+      <c r="D87" s="6"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A88" s="15"/>
+      <c r="B88" s="16"/>
+      <c r="C88" s="16"/>
+      <c r="D88" s="6"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A89" s="15"/>
+      <c r="B89" s="16"/>
+      <c r="C89" s="16"/>
+      <c r="D89" s="6"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A90" s="15"/>
+      <c r="B90" s="16"/>
+      <c r="C90" s="16"/>
+      <c r="D90" s="6"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A91" s="15"/>
+      <c r="B91" s="16"/>
+      <c r="C91" s="16"/>
+      <c r="D91" s="6"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A92" s="15"/>
+      <c r="B92" s="16"/>
+      <c r="C92" s="16"/>
+      <c r="D92" s="6"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A93" s="15"/>
+      <c r="B93" s="16"/>
+      <c r="C93" s="16"/>
+      <c r="D93" s="6"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A94" s="15"/>
+      <c r="B94" s="16"/>
+      <c r="C94" s="16"/>
+      <c r="D94" s="6"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A95" s="15"/>
+      <c r="B95" s="16"/>
+      <c r="C95" s="16"/>
+      <c r="D95" s="6"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A96" s="15"/>
+      <c r="B96" s="16"/>
+      <c r="C96" s="16"/>
+      <c r="D96" s="6"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A97" s="15"/>
+      <c r="B97" s="16"/>
+      <c r="C97" s="16"/>
+      <c r="D97" s="6"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A98" s="15"/>
+      <c r="B98" s="16"/>
+      <c r="C98" s="16"/>
+      <c r="D98" s="6"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A99" s="15"/>
+      <c r="B99" s="16"/>
+      <c r="C99" s="16"/>
+      <c r="D99" s="6"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A100" s="15"/>
+      <c r="B100" s="16"/>
+      <c r="C100" s="16"/>
+      <c r="D100" s="6"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A101" s="15"/>
+      <c r="B101" s="16"/>
+      <c r="C101" s="16"/>
+      <c r="D101" s="6"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A102" s="15"/>
+      <c r="B102" s="16"/>
+      <c r="C102" s="16"/>
+      <c r="D102" s="6"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A103" s="15"/>
+      <c r="B103" s="16"/>
+      <c r="C103" s="16"/>
+      <c r="D103" s="6"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A104" s="15"/>
+      <c r="B104" s="16"/>
+      <c r="C104" s="16"/>
+      <c r="D104" s="6"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A105" s="15"/>
+      <c r="B105" s="16"/>
+      <c r="C105" s="16"/>
+      <c r="D105" s="6"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A106" s="15"/>
+      <c r="B106" s="16"/>
+      <c r="C106" s="16"/>
+      <c r="D106" s="6"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A107" s="15"/>
+      <c r="B107" s="16"/>
+      <c r="C107" s="16"/>
+      <c r="D107" s="6"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A108" s="15"/>
+      <c r="B108" s="16"/>
+      <c r="C108" s="16"/>
+      <c r="D108" s="6"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A109" s="15"/>
+      <c r="B109" s="16"/>
+      <c r="C109" s="16"/>
+      <c r="D109" s="6"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A110" s="15"/>
+      <c r="B110" s="16"/>
+      <c r="C110" s="16"/>
+      <c r="D110" s="6"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A111" s="15"/>
+      <c r="B111" s="16"/>
+      <c r="C111" s="16"/>
+      <c r="D111" s="6"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A112" s="15"/>
+      <c r="B112" s="16"/>
+      <c r="C112" s="16"/>
+      <c r="D112" s="6"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A113" s="15"/>
+      <c r="B113" s="16"/>
+      <c r="C113" s="16"/>
+      <c r="D113" s="6"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A114" s="15"/>
+      <c r="B114" s="16"/>
+      <c r="C114" s="16"/>
+      <c r="D114" s="6"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A115" s="15"/>
+      <c r="B115" s="16"/>
+      <c r="C115" s="16"/>
+      <c r="D115" s="6"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A116" s="15"/>
+      <c r="B116" s="16"/>
+      <c r="C116" s="16"/>
+      <c r="D116" s="6"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A117" s="15"/>
+      <c r="B117" s="16"/>
+      <c r="C117" s="16"/>
+      <c r="D117" s="6"/>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A118" s="15"/>
+      <c r="B118" s="16"/>
+      <c r="C118" s="16"/>
+      <c r="D118" s="6"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A119" s="15"/>
+      <c r="B119" s="16"/>
+      <c r="C119" s="16"/>
+      <c r="D119" s="6"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A120" s="15"/>
+      <c r="B120" s="16"/>
+      <c r="C120" s="16"/>
+      <c r="D120" s="6"/>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A121" s="15"/>
+      <c r="B121" s="16"/>
+      <c r="C121" s="16"/>
+      <c r="D121" s="6"/>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A122" s="15"/>
+      <c r="B122" s="16"/>
+      <c r="C122" s="16"/>
+      <c r="D122" s="6"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A123" s="15"/>
+      <c r="B123" s="16"/>
+      <c r="C123" s="16"/>
+      <c r="D123" s="6"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A124" s="15"/>
+      <c r="B124" s="16"/>
+      <c r="C124" s="16"/>
+      <c r="D124" s="6"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A125" s="15"/>
+      <c r="B125" s="16"/>
+      <c r="C125" s="16"/>
+      <c r="D125" s="6"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A126" s="15"/>
+      <c r="B126" s="16"/>
+      <c r="C126" s="16"/>
+      <c r="D126" s="6"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A127" s="15"/>
+      <c r="B127" s="16"/>
+      <c r="C127" s="16"/>
+      <c r="D127" s="6"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A128" s="15"/>
+      <c r="B128" s="16"/>
+      <c r="C128" s="16"/>
+      <c r="D128" s="6"/>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A129" s="15"/>
+      <c r="B129" s="16"/>
+      <c r="C129" s="16"/>
+      <c r="D129" s="6"/>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A130" s="15"/>
+      <c r="B130" s="16"/>
+      <c r="C130" s="16"/>
+      <c r="D130" s="6"/>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A131" s="15"/>
+      <c r="B131" s="16"/>
+      <c r="C131" s="16"/>
+      <c r="D131" s="6"/>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A132" s="15"/>
+      <c r="B132" s="16"/>
+      <c r="C132" s="16"/>
+      <c r="D132" s="6"/>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A133" s="15"/>
+      <c r="B133" s="16"/>
+      <c r="C133" s="16"/>
+      <c r="D133" s="6"/>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A134" s="15"/>
+      <c r="B134" s="16"/>
+      <c r="C134" s="16"/>
+      <c r="D134" s="6"/>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A135" s="15"/>
+      <c r="B135" s="16"/>
+      <c r="C135" s="16"/>
+      <c r="D135" s="6"/>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A136" s="15"/>
+      <c r="B136" s="16"/>
+      <c r="C136" s="16"/>
+      <c r="D136" s="6"/>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A137" s="15"/>
+      <c r="B137" s="16"/>
+      <c r="C137" s="16"/>
+      <c r="D137" s="6"/>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A138" s="15"/>
+      <c r="B138" s="16"/>
+      <c r="C138" s="16"/>
+      <c r="D138" s="6"/>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A139" s="15"/>
+      <c r="B139" s="16"/>
+      <c r="C139" s="16"/>
+      <c r="D139" s="6"/>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A140" s="15"/>
+      <c r="B140" s="16"/>
+      <c r="C140" s="16"/>
+      <c r="D140" s="6"/>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A141" s="15"/>
+      <c r="B141" s="16"/>
+      <c r="C141" s="16"/>
+      <c r="D141" s="6"/>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A142" s="15"/>
+      <c r="B142" s="16"/>
+      <c r="C142" s="16"/>
+      <c r="D142" s="6"/>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A143" s="15"/>
+      <c r="B143" s="16"/>
+      <c r="C143" s="16"/>
+      <c r="D143" s="6"/>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A144" s="15"/>
+      <c r="B144" s="16"/>
+      <c r="C144" s="16"/>
+      <c r="D144" s="6"/>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A145" s="15"/>
+      <c r="B145" s="16"/>
+      <c r="C145" s="16"/>
+      <c r="D145" s="6"/>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A146" s="15"/>
+      <c r="B146" s="16"/>
+      <c r="C146" s="16"/>
+      <c r="D146" s="6"/>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A147" s="15"/>
+      <c r="B147" s="16"/>
+      <c r="C147" s="16"/>
+      <c r="D147" s="6"/>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A148" s="15"/>
+      <c r="B148" s="16"/>
+      <c r="C148" s="16"/>
+      <c r="D148" s="6"/>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A149" s="15"/>
+      <c r="B149" s="16"/>
+      <c r="C149" s="16"/>
+      <c r="D149" s="6"/>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A150" s="15"/>
+      <c r="B150" s="16"/>
+      <c r="C150" s="16"/>
+      <c r="D150" s="6"/>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A151" s="15"/>
+      <c r="B151" s="16"/>
+      <c r="C151" s="16"/>
+      <c r="D151" s="6"/>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A152" s="15"/>
+      <c r="B152" s="16"/>
+      <c r="C152" s="16"/>
+      <c r="D152" s="6"/>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A153" s="15"/>
+      <c r="B153" s="16"/>
+      <c r="C153" s="16"/>
+      <c r="D153" s="6"/>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A154" s="15"/>
+      <c r="B154" s="16"/>
+      <c r="C154" s="16"/>
+      <c r="D154" s="6"/>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A155" s="15"/>
+      <c r="B155" s="16"/>
+      <c r="C155" s="16"/>
+      <c r="D155" s="6"/>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A156" s="15"/>
+      <c r="B156" s="16"/>
+      <c r="C156" s="16"/>
+      <c r="D156" s="6"/>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A157" s="15"/>
+      <c r="B157" s="16"/>
+      <c r="C157" s="16"/>
+      <c r="D157" s="6"/>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A158" s="15"/>
+      <c r="B158" s="16"/>
+      <c r="C158" s="16"/>
+      <c r="D158" s="6"/>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A159" s="15"/>
+      <c r="B159" s="16"/>
+      <c r="C159" s="16"/>
+      <c r="D159" s="6"/>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A160" s="15"/>
+      <c r="B160" s="16"/>
+      <c r="C160" s="16"/>
+      <c r="D160" s="6"/>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A161" s="15"/>
+      <c r="B161" s="16"/>
+      <c r="C161" s="16"/>
+      <c r="D161" s="6"/>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A162" s="15"/>
+      <c r="B162" s="16"/>
+      <c r="C162" s="16"/>
+      <c r="D162" s="6"/>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A163" s="15"/>
+      <c r="B163" s="16"/>
+      <c r="C163" s="16"/>
+      <c r="D163" s="6"/>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A164" s="15"/>
+      <c r="B164" s="16"/>
+      <c r="C164" s="16"/>
+      <c r="D164" s="6"/>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A165" s="15"/>
+      <c r="B165" s="16"/>
+      <c r="C165" s="16"/>
+      <c r="D165" s="6"/>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A166" s="15"/>
+      <c r="B166" s="16"/>
+      <c r="C166" s="16"/>
+      <c r="D166" s="6"/>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A167" s="15"/>
+      <c r="B167" s="16"/>
+      <c r="C167" s="16"/>
+      <c r="D167" s="6"/>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A168" s="15"/>
+      <c r="B168" s="16"/>
+      <c r="C168" s="16"/>
+      <c r="D168" s="6"/>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A169" s="15"/>
+      <c r="B169" s="16"/>
+      <c r="C169" s="16"/>
+      <c r="D169" s="6"/>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A170" s="15"/>
+      <c r="B170" s="16"/>
+      <c r="C170" s="16"/>
+      <c r="D170" s="6"/>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A171" s="15"/>
+      <c r="B171" s="16"/>
+      <c r="C171" s="16"/>
+      <c r="D171" s="6"/>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A172" s="15"/>
+      <c r="B172" s="16"/>
+      <c r="C172" s="16"/>
+      <c r="D172" s="6"/>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A173" s="15"/>
+      <c r="B173" s="16"/>
+      <c r="C173" s="16"/>
+      <c r="D173" s="6"/>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A174" s="15"/>
+      <c r="B174" s="16"/>
+      <c r="C174" s="16"/>
+      <c r="D174" s="6"/>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A175" s="15"/>
+      <c r="B175" s="16"/>
+      <c r="C175" s="16"/>
+      <c r="D175" s="6"/>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A176" s="15"/>
+      <c r="B176" s="16"/>
+      <c r="C176" s="16"/>
+      <c r="D176" s="6"/>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A177" s="15"/>
+      <c r="B177" s="16"/>
+      <c r="C177" s="16"/>
+      <c r="D177" s="6"/>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A178" s="15"/>
+      <c r="B178" s="16"/>
+      <c r="C178" s="16"/>
+      <c r="D178" s="6"/>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A179" s="15"/>
+      <c r="B179" s="16"/>
+      <c r="C179" s="16"/>
+      <c r="D179" s="6"/>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A180" s="15"/>
+      <c r="B180" s="16"/>
+      <c r="C180" s="16"/>
+      <c r="D180" s="6"/>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A181" s="15"/>
+      <c r="B181" s="16"/>
+      <c r="C181" s="16"/>
+      <c r="D181" s="6"/>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A182" s="15"/>
+      <c r="B182" s="16"/>
+      <c r="C182" s="16"/>
+      <c r="D182" s="6"/>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A183" s="15"/>
+      <c r="B183" s="16"/>
+      <c r="C183" s="16"/>
+      <c r="D183" s="6"/>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A184" s="15"/>
+      <c r="B184" s="16"/>
+      <c r="C184" s="16"/>
+      <c r="D184" s="6"/>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A185" s="15"/>
+      <c r="B185" s="16"/>
+      <c r="C185" s="16"/>
+      <c r="D185" s="6"/>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A186" s="15"/>
+      <c r="B186" s="16"/>
+      <c r="C186" s="16"/>
+      <c r="D186" s="6"/>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A187" s="15"/>
+      <c r="B187" s="16"/>
+      <c r="C187" s="16"/>
+      <c r="D187" s="6"/>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A188" s="15"/>
+      <c r="B188" s="16"/>
+      <c r="C188" s="16"/>
+      <c r="D188" s="6"/>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A189" s="15"/>
+      <c r="B189" s="16"/>
+      <c r="C189" s="16"/>
+      <c r="D189" s="6"/>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A190" s="15"/>
+      <c r="B190" s="16"/>
+      <c r="C190" s="16"/>
+      <c r="D190" s="6"/>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A191" s="15"/>
+      <c r="B191" s="16"/>
+      <c r="C191" s="16"/>
+      <c r="D191" s="6"/>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A192" s="15"/>
+      <c r="B192" s="16"/>
+      <c r="C192" s="16"/>
+      <c r="D192" s="6"/>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A193" s="15"/>
+      <c r="B193" s="16"/>
+      <c r="C193" s="16"/>
+      <c r="D193" s="6"/>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A194" s="15"/>
+      <c r="B194" s="16"/>
+      <c r="C194" s="16"/>
+      <c r="D194" s="6"/>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A195" s="15"/>
+      <c r="B195" s="16"/>
+      <c r="C195" s="16"/>
+      <c r="D195" s="6"/>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A196" s="15"/>
+      <c r="B196" s="16"/>
+      <c r="C196" s="16"/>
+      <c r="D196" s="6"/>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A197" s="15"/>
+      <c r="B197" s="16"/>
+      <c r="C197" s="16"/>
+      <c r="D197" s="6"/>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A198" s="15"/>
+      <c r="B198" s="16"/>
+      <c r="C198" s="16"/>
+      <c r="D198" s="6"/>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A199" s="15"/>
+      <c r="B199" s="16"/>
+      <c r="C199" s="16"/>
+      <c r="D199" s="6"/>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A200" s="15"/>
+      <c r="B200" s="16"/>
+      <c r="C200" s="16"/>
+      <c r="D200" s="6"/>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A201" s="15"/>
+      <c r="B201" s="16"/>
+      <c r="C201" s="16"/>
+      <c r="D201" s="6"/>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A202" s="15"/>
+      <c r="B202" s="16"/>
+      <c r="C202" s="16"/>
+      <c r="D202" s="6"/>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A203" s="4"/>
+      <c r="B203" s="5"/>
+      <c r="C203" s="5"/>
+      <c r="D203" s="6"/>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A204" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B204" s="2"/>
+      <c r="C204" s="2">
         <v>1895.62</v>
       </c>
-      <c r="D48" s="3"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="8"/>
-      <c r="B49" s="5" t="s">
+      <c r="D204" s="3"/>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A205" s="8"/>
+      <c r="B205" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C205" s="5">
         <v>1047.72</v>
       </c>
-      <c r="D49" s="6"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="9"/>
-      <c r="B50" s="10" t="s">
+      <c r="D205" s="6"/>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A206" s="9"/>
+      <c r="B206" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C50" s="10">
+      <c r="C206" s="10">
         <v>847.9</v>
       </c>
-      <c r="D50" s="11"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="12"/>
-      <c r="B51" s="13" t="s">
+      <c r="D206" s="11"/>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A207" s="12"/>
+      <c r="B207" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C51" s="13">
+      <c r="C207" s="13">
         <v>17850</v>
       </c>
-      <c r="D51" s="14"/>
-    </row>
-    <row r="2656" spans="3:3" x14ac:dyDescent="0.15">
-      <c r="C2656" t="s">
+      <c r="D207" s="14"/>
+    </row>
+    <row r="2812" spans="3:3" x14ac:dyDescent="0.15">
+      <c r="C2812" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D51"/>
+  <autoFilter ref="A1:D207"/>
   <mergeCells count="6">
     <mergeCell ref="A2:A25"/>
     <mergeCell ref="B9:B11"/>

</xml_diff>